<commit_message>
starting to change function for prepare for prototype and classes create
</commit_message>
<xml_diff>
--- a/список.xlsx
+++ b/список.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="13335" windowHeight="6150"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="13335" windowHeight="6150" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="функции" sheetId="1" r:id="rId1"/>
     <sheet name="тэги" sheetId="2" r:id="rId2"/>
     <sheet name="неглобальные пееременные" sheetId="4" r:id="rId3"/>
+    <sheet name="Лист1" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
   <si>
     <t>Функция</t>
   </si>
@@ -148,13 +149,58 @@
   </si>
   <si>
     <t>описание</t>
+  </si>
+  <si>
+    <t>строка названия листа</t>
+  </si>
+  <si>
+    <t>помещение в верстку</t>
+  </si>
+  <si>
+    <t>корректировка (вытаскивает значение из инпута, заменяет блоком, меняет надпись на кнопке, удаляет изначальный блок или обратно)</t>
+  </si>
+  <si>
+    <t>строка задачи</t>
+  </si>
+  <si>
+    <t>название объекта</t>
+  </si>
+  <si>
+    <t>функция</t>
+  </si>
+  <si>
+    <t>кнопка вывода листа</t>
+  </si>
+  <si>
+    <t>конструктор (блок, инпут и кнопка)</t>
+  </si>
+  <si>
+    <t>строка добавления задачи</t>
+  </si>
+  <si>
+    <t>inputStringConstructor конструктор (блок, инпут и кнопка)</t>
+  </si>
+  <si>
+    <t>placeInDocument помещение в верстку</t>
+  </si>
+  <si>
+    <t>addTask добавление нового элемента</t>
+  </si>
+  <si>
+    <t>correct корректировка (вытаскивает значение из инпута, заменяет блоком, меняет надпись на кнопке, удаляет изначальный блок или обратно)</t>
+  </si>
+  <si>
+    <t>deleteTask удаление (создание кнопки, помещение в верстку, присвоение функции удаления при нажатии)</t>
+  </si>
+  <si>
+    <t>getList получает значение всех задач и вывоит в алерт</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,8 +233,17 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,8 +262,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -268,11 +329,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -289,35 +365,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="255" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="255"/>
@@ -333,6 +385,39 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -674,16 +759,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" style="8" customWidth="1"/>
     <col min="2" max="2" width="29" style="5" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="28" style="5" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" style="2" customWidth="1"/>
@@ -692,7 +777,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -701,7 +786,7 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="11" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -716,14 +801,14 @@
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" ht="45">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="18" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="6"/>
-      <c r="D2" s="20"/>
+      <c r="D2" s="12"/>
       <c r="E2" s="3" t="s">
         <v>23</v>
       </c>
@@ -738,14 +823,14 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="9"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="21"/>
+      <c r="D3" s="13"/>
       <c r="E3" s="3" t="s">
         <v>24</v>
       </c>
@@ -760,15 +845,15 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="136.5">
-      <c r="A4" s="9"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="22" t="s">
+      <c r="C4" s="22"/>
+      <c r="D4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="10" t="s">
         <v>28</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -778,12 +863,12 @@
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" ht="30">
-      <c r="A5" s="9"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="14"/>
       <c r="E5" s="3"/>
       <c r="F5" s="4" t="s">
         <v>14</v>
@@ -792,12 +877,12 @@
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="10"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="15"/>
       <c r="E6" s="3"/>
       <c r="F6" s="4" t="s">
         <v>15</v>
@@ -805,16 +890,16 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="196.5">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="18" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="13" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="3"/>
@@ -825,12 +910,12 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="30">
-      <c r="A8" s="10"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="15"/>
       <c r="E8" s="3"/>
       <c r="F8" s="4" t="s">
         <v>21</v>
@@ -839,19 +924,19 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="181.5">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="24" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="10" t="s">
         <v>28</v>
       </c>
       <c r="F9" s="4" t="s">
@@ -861,12 +946,12 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" ht="45">
-      <c r="A10" s="12"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="15"/>
       <c r="E10" s="3"/>
       <c r="F10" s="4" t="s">
         <v>22</v>
@@ -878,7 +963,7 @@
       <c r="A11" s="7"/>
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="24"/>
+      <c r="D11" s="16"/>
       <c r="E11" s="3"/>
       <c r="F11" s="4"/>
       <c r="G11" s="3"/>
@@ -888,7 +973,7 @@
       <c r="A12" s="7"/>
       <c r="B12" s="4"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="24"/>
+      <c r="D12" s="16"/>
       <c r="E12" s="3"/>
       <c r="F12" s="4"/>
       <c r="G12" s="3"/>
@@ -898,7 +983,7 @@
       <c r="A13" s="7"/>
       <c r="B13" s="4"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="24"/>
+      <c r="D13" s="16"/>
       <c r="E13" s="3"/>
       <c r="F13" s="4"/>
       <c r="G13" s="3"/>
@@ -908,7 +993,7 @@
       <c r="A14" s="7"/>
       <c r="B14" s="4"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="24"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="3"/>
       <c r="F14" s="4"/>
       <c r="G14" s="3"/>
@@ -918,7 +1003,7 @@
       <c r="A15" s="7"/>
       <c r="B15" s="4"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="24"/>
+      <c r="D15" s="16"/>
       <c r="E15" s="3"/>
       <c r="F15" s="4"/>
       <c r="G15" s="3"/>
@@ -928,7 +1013,7 @@
       <c r="A16" s="7"/>
       <c r="B16" s="4"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="24"/>
+      <c r="D16" s="16"/>
       <c r="E16" s="3"/>
       <c r="F16" s="4"/>
       <c r="G16" s="3"/>
@@ -938,7 +1023,7 @@
       <c r="A17" s="7"/>
       <c r="B17" s="4"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="24"/>
+      <c r="D17" s="16"/>
       <c r="E17" s="3"/>
       <c r="F17" s="4"/>
       <c r="G17" s="3"/>
@@ -948,7 +1033,7 @@
       <c r="A18" s="7"/>
       <c r="B18" s="4"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="24"/>
+      <c r="D18" s="16"/>
       <c r="E18" s="3"/>
       <c r="F18" s="4"/>
       <c r="G18" s="3"/>
@@ -958,7 +1043,7 @@
       <c r="A19" s="7"/>
       <c r="B19" s="4"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="24"/>
+      <c r="D19" s="16"/>
       <c r="E19" s="3"/>
       <c r="F19" s="4"/>
       <c r="G19" s="3"/>
@@ -968,7 +1053,7 @@
       <c r="A20" s="7"/>
       <c r="B20" s="4"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="24"/>
+      <c r="D20" s="16"/>
       <c r="E20" s="3"/>
       <c r="F20" s="4"/>
       <c r="G20" s="3"/>
@@ -978,7 +1063,7 @@
       <c r="A21" s="7"/>
       <c r="B21" s="4"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="24"/>
+      <c r="D21" s="16"/>
       <c r="E21" s="3"/>
       <c r="F21" s="4"/>
       <c r="G21" s="3"/>
@@ -1111,4 +1196,102 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="30">
+      <c r="A1" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="45">
+      <c r="A2" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30">
+      <c r="A3" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="27"/>
+    </row>
+    <row r="4" spans="1:5" ht="90">
+      <c r="A4" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="27"/>
+    </row>
+    <row r="5" spans="1:5" ht="75">
+      <c r="A5" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>